<commit_message>
changes to alot of things
</commit_message>
<xml_diff>
--- a/Case Study/Subnet Planning.xlsx
+++ b/Case Study/Subnet Planning.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gamal\Documents\Uni\BA-CS\Year 2 Semester 1\TNE20002\Case Study\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01039F60-69DE-4EA2-9052-1EC596D3B2CA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18023145-EBA9-4137-97BE-DFA5CADCDE82}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="36000" yWindow="3735" windowWidth="21600" windowHeight="11385" xr2:uid="{43D89B2B-CCA6-46CA-87E2-CB9722D36B79}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{43D89B2B-CCA6-46CA-87E2-CB9722D36B79}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="72">
   <si>
     <t>VLAN NAME</t>
   </si>
@@ -222,6 +222,33 @@
   </si>
   <si>
     <t>68.32.7.97</t>
+  </si>
+  <si>
+    <t>68.32.3.1</t>
+  </si>
+  <si>
+    <t>255.255.255.224</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 68.32.7.161</t>
+  </si>
+  <si>
+    <t>68.32.7.177</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 68.32.7.193</t>
+  </si>
+  <si>
+    <t>68.32.7.233</t>
+  </si>
+  <si>
+    <t>68.32.6.193</t>
+  </si>
+  <si>
+    <t>Start Port</t>
+  </si>
+  <si>
+    <t>End Port</t>
   </si>
 </sst>
 </file>
@@ -261,7 +288,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -282,17 +309,6 @@
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
       <diagonal/>
     </border>
     <border>
@@ -366,7 +382,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -381,17 +397,17 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
@@ -403,14 +419,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -729,8 +749,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5613AE56-6E6A-48B0-ADC8-3EE92C78B678}">
   <dimension ref="A1:O33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="E31" sqref="E31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -748,24 +768,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="10"/>
-      <c r="C1" s="10"/>
-      <c r="D1" s="10"/>
-      <c r="E1" s="10"/>
-      <c r="H1" s="16" t="s">
+      <c r="B1" s="9"/>
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
+      <c r="E1" s="9"/>
+      <c r="H1" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="I1" s="14"/>
-      <c r="J1" s="14"/>
-      <c r="K1" s="14"/>
-      <c r="M1" s="11" t="s">
+      <c r="I1" s="13"/>
+      <c r="J1" s="13"/>
+      <c r="K1" s="13"/>
+      <c r="M1" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="N1" s="12"/>
-      <c r="O1" s="13"/>
+      <c r="N1" s="11"/>
+      <c r="O1" s="12"/>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
@@ -816,10 +836,10 @@
         <f>(B3*1.33)</f>
         <v>166.25</v>
       </c>
-      <c r="D3" s="8" t="s">
+      <c r="D3" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="E3" s="8" t="s">
+      <c r="E3" s="7" t="s">
         <v>36</v>
       </c>
       <c r="H3" s="1" t="s">
@@ -856,10 +876,10 @@
         <f t="shared" ref="C4:C8" si="0">(B4*1.33)</f>
         <v>239.4</v>
       </c>
-      <c r="D4" s="8" t="s">
+      <c r="D4" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="E4" s="8" t="s">
+      <c r="E4" s="7" t="s">
         <v>36</v>
       </c>
       <c r="H4" s="1" t="s">
@@ -896,10 +916,10 @@
         <f t="shared" si="0"/>
         <v>266</v>
       </c>
-      <c r="D5" s="8" t="s">
+      <c r="D5" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="E5" s="8" t="s">
+      <c r="E5" s="7" t="s">
         <v>40</v>
       </c>
       <c r="H5" s="1" t="s">
@@ -936,10 +956,10 @@
         <f t="shared" si="0"/>
         <v>6.65</v>
       </c>
-      <c r="D6" s="8" t="s">
+      <c r="D6" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="E6" s="8" t="s">
+      <c r="E6" s="7" t="s">
         <v>41</v>
       </c>
       <c r="H6" s="1" t="s">
@@ -976,10 +996,10 @@
         <f t="shared" si="0"/>
         <v>6.65</v>
       </c>
-      <c r="D7" s="8" t="s">
+      <c r="D7" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="E7" s="8" t="s">
+      <c r="E7" s="7" t="s">
         <v>41</v>
       </c>
       <c r="H7" s="1" t="s">
@@ -1016,10 +1036,10 @@
         <f t="shared" si="0"/>
         <v>6.65</v>
       </c>
-      <c r="D8" s="8" t="s">
+      <c r="D8" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="E8" s="8" t="s">
+      <c r="E8" s="7" t="s">
         <v>41</v>
       </c>
       <c r="H8" s="1" t="s">
@@ -1057,10 +1077,10 @@
         <f>(B9*2)</f>
         <v>4</v>
       </c>
-      <c r="D9" s="8" t="s">
+      <c r="D9" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="E9" s="8" t="s">
+      <c r="E9" s="7" t="s">
         <v>45</v>
       </c>
       <c r="H9" s="1" t="s">
@@ -1082,7 +1102,7 @@
         <f>SUM(N3:N7)</f>
         <v>142</v>
       </c>
-      <c r="O9" s="7">
+      <c r="O9" s="6">
         <f>SUM(O3:O7)</f>
         <v>190.20000000000002</v>
       </c>
@@ -1099,10 +1119,10 @@
         <f>(C11/24)+2</f>
         <v>30.983333333333331</v>
       </c>
-      <c r="D10" s="8" t="s">
+      <c r="D10" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="E10" s="8" t="s">
+      <c r="E10" s="7" t="s">
         <v>47</v>
       </c>
       <c r="H10" s="3" t="s">
@@ -1131,8 +1151,8 @@
         <f>SUM(C3:C9)</f>
         <v>695.59999999999991</v>
       </c>
-      <c r="D11" s="8"/>
-      <c r="E11" s="8"/>
+      <c r="D11" s="7"/>
+      <c r="E11" s="7"/>
       <c r="H11" s="3" t="s">
         <v>11</v>
       </c>
@@ -1144,22 +1164,24 @@
       <c r="K11" s="5"/>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A13" s="16" t="s">
+      <c r="A13" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="B13" s="14"/>
-      <c r="C13" s="14"/>
-      <c r="D13" s="14"/>
-      <c r="E13" s="14"/>
-      <c r="H13" s="15" t="s">
+      <c r="B13" s="13"/>
+      <c r="C13" s="13"/>
+      <c r="D13" s="13"/>
+      <c r="E13" s="13"/>
+      <c r="H13" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="I13" s="15"/>
-      <c r="J13" s="15"/>
-      <c r="N13" s="14" t="s">
+      <c r="I13" s="11"/>
+      <c r="J13" s="11"/>
+      <c r="K13" s="11"/>
+      <c r="L13" s="12"/>
+      <c r="N13" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="O13" s="14"/>
+      <c r="O13" s="13"/>
     </row>
     <row r="14" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
@@ -1186,6 +1208,12 @@
       <c r="J14" s="1" t="s">
         <v>21</v>
       </c>
+      <c r="K14" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="L14" s="3" t="s">
+        <v>31</v>
+      </c>
       <c r="N14" s="1" t="s">
         <v>28</v>
       </c>
@@ -1220,6 +1248,12 @@
         <f>I15*1.33</f>
         <v>186.20000000000002</v>
       </c>
+      <c r="K15" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="L15" s="5" t="s">
+        <v>36</v>
+      </c>
       <c r="N15" s="1" t="s">
         <v>27</v>
       </c>
@@ -1254,6 +1288,12 @@
         <f t="shared" ref="J16:J20" si="3">I16*1.33</f>
         <v>6.65</v>
       </c>
+      <c r="K16" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="L16" s="5" t="s">
+        <v>41</v>
+      </c>
       <c r="N16" s="1" t="s">
         <v>24</v>
       </c>
@@ -1288,6 +1328,12 @@
         <f t="shared" si="3"/>
         <v>6.65</v>
       </c>
+      <c r="K17" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="L17" s="5" t="s">
+        <v>41</v>
+      </c>
       <c r="N17" s="1" t="s">
         <v>22</v>
       </c>
@@ -1322,6 +1368,12 @@
         <f t="shared" si="3"/>
         <v>6.65</v>
       </c>
+      <c r="K18" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="L18" s="5" t="s">
+        <v>41</v>
+      </c>
       <c r="N18" s="1" t="s">
         <v>12</v>
       </c>
@@ -1356,6 +1408,12 @@
         <f>I19*2</f>
         <v>4</v>
       </c>
+      <c r="K19" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="L19" s="5" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
@@ -1375,16 +1433,18 @@
       <c r="E20" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="H20" s="6" t="s">
+      <c r="H20" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="I20" s="6">
+      <c r="I20" s="3">
         <v>3</v>
       </c>
       <c r="J20" s="2">
         <f t="shared" si="3"/>
         <v>3.99</v>
       </c>
+      <c r="K20" s="5"/>
+      <c r="L20" s="5"/>
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
@@ -1394,7 +1454,7 @@
         <f>SUM(B15:B19)</f>
         <v>97</v>
       </c>
-      <c r="C21" s="7">
+      <c r="C21" s="6">
         <f>SUM(C15:C19)</f>
         <v>130.35000000000002</v>
       </c>
@@ -1411,6 +1471,12 @@
         <f>(J22/24)+3+J20</f>
         <v>15.746250000000002</v>
       </c>
+      <c r="K21" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="L21" s="5" t="s">
+        <v>64</v>
+      </c>
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.25">
       <c r="H22" s="3" t="s">
@@ -1420,10 +1486,12 @@
         <f>SUM(I15:I19)</f>
         <v>157</v>
       </c>
-      <c r="J22" s="7">
+      <c r="J22" s="6">
         <f>SUM(J15:J19)</f>
         <v>210.15000000000003</v>
       </c>
+      <c r="K22" s="5"/>
+      <c r="L22" s="5"/>
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
@@ -1432,6 +1500,12 @@
       <c r="B24" s="1" t="s">
         <v>32</v>
       </c>
+      <c r="C24" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="D24" s="5" t="s">
+        <v>71</v>
+      </c>
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
@@ -1440,6 +1514,12 @@
       <c r="B25" s="1">
         <v>10</v>
       </c>
+      <c r="C25" s="17">
+        <v>1</v>
+      </c>
+      <c r="D25" s="6">
+        <v>3</v>
+      </c>
     </row>
     <row r="26" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
@@ -1448,6 +1528,12 @@
       <c r="B26" s="1">
         <v>20</v>
       </c>
+      <c r="C26" s="17">
+        <v>4</v>
+      </c>
+      <c r="D26" s="6">
+        <v>6</v>
+      </c>
     </row>
     <row r="27" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
@@ -1456,6 +1542,12 @@
       <c r="B27" s="1">
         <v>30</v>
       </c>
+      <c r="C27" s="18">
+        <v>7</v>
+      </c>
+      <c r="D27" s="6">
+        <v>9</v>
+      </c>
     </row>
     <row r="28" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
@@ -1464,6 +1556,12 @@
       <c r="B28" s="1">
         <v>40</v>
       </c>
+      <c r="C28" s="17">
+        <v>10</v>
+      </c>
+      <c r="D28" s="6">
+        <v>12</v>
+      </c>
     </row>
     <row r="29" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
@@ -1472,6 +1570,12 @@
       <c r="B29" s="1">
         <v>50</v>
       </c>
+      <c r="C29" s="17">
+        <v>13</v>
+      </c>
+      <c r="D29" s="6">
+        <v>15</v>
+      </c>
     </row>
     <row r="30" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
@@ -1480,6 +1584,12 @@
       <c r="B30" s="1">
         <v>60</v>
       </c>
+      <c r="C30" s="17">
+        <v>16</v>
+      </c>
+      <c r="D30" s="6">
+        <v>18</v>
+      </c>
     </row>
     <row r="31" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
@@ -1488,6 +1598,12 @@
       <c r="B31" s="1">
         <v>70</v>
       </c>
+      <c r="C31" s="17">
+        <v>19</v>
+      </c>
+      <c r="D31" s="6">
+        <v>21</v>
+      </c>
     </row>
     <row r="32" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
@@ -1496,23 +1612,31 @@
       <c r="B32" s="1">
         <v>80</v>
       </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C32" s="17">
+        <v>22</v>
+      </c>
+      <c r="D32" s="6">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>10</v>
       </c>
       <c r="B33" s="1">
         <v>33</v>
       </c>
+      <c r="C33" s="15"/>
+      <c r="D33" s="16"/>
     </row>
   </sheetData>
   <mergeCells count="6">
     <mergeCell ref="A1:E1"/>
     <mergeCell ref="M1:O1"/>
     <mergeCell ref="N13:O13"/>
-    <mergeCell ref="H13:J13"/>
     <mergeCell ref="H1:K1"/>
     <mergeCell ref="A13:E13"/>
+    <mergeCell ref="H13:L13"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>